<commit_message>
minor updates to the worksheets
</commit_message>
<xml_diff>
--- a/test/samples/test_sample.xlsx
+++ b/test/samples/test_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yacintmimi/Documents/UVM/Fall 2017/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yacintmimi/Documents/UVM/Fall 2017/ma_option_vol/test/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DBA5B7-CEC8-5E4D-BEAE-6B6E3453D969}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B801C80-C5D0-7246-ABA9-A742E04CC1B8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="940" windowWidth="25040" windowHeight="14520" xr2:uid="{047C5588-AB4A-954D-9979-596C4E0FD388}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -549,43 +549,43 @@
         <v>13</v>
       </c>
       <c r="B2" s="1">
-        <v>42331</v>
+        <v>41761</v>
       </c>
       <c r="C2" s="1">
-        <v>42466</v>
+        <v>41785</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
       </c>
       <c r="J2">
-        <v>183831.5</v>
+        <v>124564.07</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L2">
-        <v>10.69</v>
+        <v>9.93</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -593,43 +593,43 @@
         <v>13</v>
       </c>
       <c r="B3" s="1">
-        <v>41761</v>
+        <v>42331</v>
       </c>
       <c r="C3" s="1">
-        <v>41785</v>
+        <v>42466</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
       </c>
       <c r="J3">
-        <v>124564.07</v>
+        <v>183831.5</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L3">
-        <v>9.93</v>
+        <v>10.69</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -677,6 +677,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:N4">
+    <sortCondition ref="B2:B4"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>